<commit_message>
Added multithreaded processing for figure generation, docstrings, organized import block, zarr-based SA saving, cleaned up comments
</commit_message>
<xml_diff>
--- a/xlsxs/animal-to-bestdepth.xlsx
+++ b/xlsxs/animal-to-bestdepth.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\MarshMountainSort\xlsxs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\MarshMountainSort\xlsxs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71254E1-8797-49A8-A8DC-6415E9F85B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947A9260-655F-46D5-A25B-EEFDC3984105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="3690" windowWidth="21600" windowHeight="12735" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="12-04-2024" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="12-10-2024" sheetId="3" r:id="rId3"/>
     <sheet name="12-12-2024" sheetId="4" r:id="rId4"/>
     <sheet name="12-12-20241" sheetId="5" r:id="rId5"/>
-    <sheet name="12-19-20241" sheetId="57" r:id="rId6"/>
+    <sheet name="12-19-20241" sheetId="6" r:id="rId6"/>
+    <sheet name="01-30-2025" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="37">
   <si>
     <t>id</t>
   </si>
@@ -130,18 +131,41 @@
   <si>
     <t>1226_Bl6 WT_6 half turns + 1-4th of a full turn_after turning_04-04-17</t>
   </si>
+  <si>
+    <t>579-WT-GCG-M-20htL-20htR tetrodes 1-22-25_250122_164354</t>
+  </si>
+  <si>
+    <t>579-WT-GCG-M-20htL-20htR tetrodes after 2nd handling 1-23-25_250123_113219</t>
+  </si>
+  <si>
+    <t>580-WT-GCG-M-20htL-20htR tetrodes 1-22-25_250122_164354</t>
+  </si>
+  <si>
+    <t>580-WT-GCG-M-20htL-20htR tetrodes after handling 1-23-25_250123_111523</t>
+  </si>
+  <si>
+    <t>613-WT-GCG-M-20htL-20htR tetrodes 1-29-25_250129_092654</t>
+  </si>
+  <si>
+    <t>619-WT-GCG-M-18htL-18htR tetrodes after handling 1-28-25_250128_113333</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -172,7 +196,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -240,11 +264,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -256,6 +295,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -7604,10 +7646,10 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E117"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -9119,4 +9161,1920 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E145"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>501</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>501</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>501</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>501</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>502</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>502</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>502</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>502</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>513</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>513</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>513</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>513</v>
+      </c>
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>514</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>514</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>514</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>514</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>529</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>529</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>529</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>529</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>530</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>530</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>530</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>530</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>537</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>537</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>537</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>537</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>556</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>556</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>556</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>556</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>557</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>557</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <v>557</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <v>557</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <v>579</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <v>579</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <v>579</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="E40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>579</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+      <c r="E41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="5">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>580</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+      <c r="E42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <v>580</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+      <c r="E43" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <v>580</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+      <c r="E44" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="5">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <v>580</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+      <c r="E45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <v>613</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+      <c r="E46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <v>613</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="5">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>613</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="5">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <v>613</v>
+      </c>
+      <c r="C49" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <v>619</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="5">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>619</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="5">
+        <v>50</v>
+      </c>
+      <c r="B52">
+        <v>619</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="5">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>619</v>
+      </c>
+      <c r="C53" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="5">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>766</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>766</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>3.25</v>
+      </c>
+      <c r="E55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="5">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>766</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>3.25</v>
+      </c>
+      <c r="E56" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="5">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>766</v>
+      </c>
+      <c r="C57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="5">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>1131</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>1131</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="5">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>1131</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="5">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>1131</v>
+      </c>
+      <c r="C61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="5">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>1132</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="5">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>1132</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>1132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="5">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>1132</v>
+      </c>
+      <c r="C65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>1133</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66">
+        <v>2.75</v>
+      </c>
+      <c r="E66" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="5">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>1133</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67">
+        <v>2.75</v>
+      </c>
+      <c r="E67" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>1133</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="5">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>1133</v>
+      </c>
+      <c r="C69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="5">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>1155</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="5">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>1155</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="5">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>1155</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>1155</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="5">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>1158</v>
+      </c>
+      <c r="C74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="5">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>1158</v>
+      </c>
+      <c r="C75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="5">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>1158</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>1158</v>
+      </c>
+      <c r="C77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="5">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>1176</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78">
+        <v>3.375</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="5">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>1176</v>
+      </c>
+      <c r="C79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="5">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>1176</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80">
+        <v>3.25</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="5">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>1176</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>1177</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="5">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>1177</v>
+      </c>
+      <c r="C83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="5">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>1177</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" s="5">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>1177</v>
+      </c>
+      <c r="C85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="5">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>1178</v>
+      </c>
+      <c r="C86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>1178</v>
+      </c>
+      <c r="C87" t="s">
+        <v>6</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+      <c r="E87" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" s="5">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>1178</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="5">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>1178</v>
+      </c>
+      <c r="C89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" s="5">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>1185</v>
+      </c>
+      <c r="C90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" s="5">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>1185</v>
+      </c>
+      <c r="C91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>1185</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" s="5">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>1185</v>
+      </c>
+      <c r="C93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94" s="5">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>1203</v>
+      </c>
+      <c r="C94" t="s">
+        <v>7</v>
+      </c>
+      <c r="D94">
+        <v>2.5</v>
+      </c>
+      <c r="E94" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95" s="5">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>1203</v>
+      </c>
+      <c r="C95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96" s="5">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>1203</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>1203</v>
+      </c>
+      <c r="C97" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="5">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>1211</v>
+      </c>
+      <c r="C98" t="s">
+        <v>7</v>
+      </c>
+      <c r="D98">
+        <v>3.25</v>
+      </c>
+      <c r="E98" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" s="5">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>1211</v>
+      </c>
+      <c r="C99" t="s">
+        <v>6</v>
+      </c>
+      <c r="D99">
+        <v>3</v>
+      </c>
+      <c r="E99" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="5">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>1211</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100">
+        <v>3.25</v>
+      </c>
+      <c r="E100" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="5">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>1211</v>
+      </c>
+      <c r="C101" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>1214</v>
+      </c>
+      <c r="C102" t="s">
+        <v>7</v>
+      </c>
+      <c r="D102">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" s="5">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>1214</v>
+      </c>
+      <c r="C103" t="s">
+        <v>6</v>
+      </c>
+      <c r="D103">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" s="5">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>1214</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="5">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>1214</v>
+      </c>
+      <c r="C105" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="5">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>1225</v>
+      </c>
+      <c r="C106" t="s">
+        <v>7</v>
+      </c>
+      <c r="D106">
+        <v>3.25</v>
+      </c>
+      <c r="E106" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
+        <v>105</v>
+      </c>
+      <c r="B107">
+        <v>1225</v>
+      </c>
+      <c r="C107" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107">
+        <v>3.25</v>
+      </c>
+      <c r="E107" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="5">
+        <v>106</v>
+      </c>
+      <c r="B108">
+        <v>1225</v>
+      </c>
+      <c r="C108" t="s">
+        <v>4</v>
+      </c>
+      <c r="D108">
+        <v>3.25</v>
+      </c>
+      <c r="E108" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="5">
+        <v>107</v>
+      </c>
+      <c r="B109">
+        <v>1225</v>
+      </c>
+      <c r="C109" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="5">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>1226</v>
+      </c>
+      <c r="C110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="5">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>1226</v>
+      </c>
+      <c r="C111" t="s">
+        <v>6</v>
+      </c>
+      <c r="D111">
+        <v>3.25</v>
+      </c>
+      <c r="E111" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" s="5">
+        <v>110</v>
+      </c>
+      <c r="B112">
+        <v>1226</v>
+      </c>
+      <c r="C112" t="s">
+        <v>4</v>
+      </c>
+      <c r="D112">
+        <v>3.25</v>
+      </c>
+      <c r="E112" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="5">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>1226</v>
+      </c>
+      <c r="C113" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="5">
+        <v>112</v>
+      </c>
+      <c r="B114">
+        <v>1227</v>
+      </c>
+      <c r="C114" t="s">
+        <v>7</v>
+      </c>
+      <c r="D114">
+        <v>3</v>
+      </c>
+      <c r="E114" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="5">
+        <v>113</v>
+      </c>
+      <c r="B115">
+        <v>1227</v>
+      </c>
+      <c r="C115" t="s">
+        <v>6</v>
+      </c>
+      <c r="D115">
+        <v>3.25</v>
+      </c>
+      <c r="E115" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="5">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>1227</v>
+      </c>
+      <c r="C116" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="5">
+        <v>115</v>
+      </c>
+      <c r="B117">
+        <v>1227</v>
+      </c>
+      <c r="C117" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="5">
+        <v>116</v>
+      </c>
+      <c r="B118">
+        <v>1231</v>
+      </c>
+      <c r="C118" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="5">
+        <v>117</v>
+      </c>
+      <c r="B119">
+        <v>1231</v>
+      </c>
+      <c r="C119" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120" s="5">
+        <v>118</v>
+      </c>
+      <c r="B120">
+        <v>1231</v>
+      </c>
+      <c r="C120" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" s="5">
+        <v>119</v>
+      </c>
+      <c r="B121">
+        <v>1231</v>
+      </c>
+      <c r="C121" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="5">
+        <v>120</v>
+      </c>
+      <c r="B122">
+        <v>1233</v>
+      </c>
+      <c r="C122" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="5">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>1233</v>
+      </c>
+      <c r="C123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="5">
+        <v>122</v>
+      </c>
+      <c r="B124">
+        <v>1233</v>
+      </c>
+      <c r="C124" t="s">
+        <v>4</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
+      </c>
+      <c r="E124" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="5">
+        <v>123</v>
+      </c>
+      <c r="B125">
+        <v>1233</v>
+      </c>
+      <c r="C125" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="5">
+        <v>124</v>
+      </c>
+      <c r="B126">
+        <v>1234</v>
+      </c>
+      <c r="C126" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126">
+        <v>3.25</v>
+      </c>
+      <c r="E126" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="5">
+        <v>125</v>
+      </c>
+      <c r="B127">
+        <v>1234</v>
+      </c>
+      <c r="C127" t="s">
+        <v>6</v>
+      </c>
+      <c r="D127">
+        <v>3</v>
+      </c>
+      <c r="E127" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A128" s="5">
+        <v>126</v>
+      </c>
+      <c r="B128">
+        <v>1234</v>
+      </c>
+      <c r="C128" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="5">
+        <v>127</v>
+      </c>
+      <c r="B129">
+        <v>1234</v>
+      </c>
+      <c r="C129" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="5">
+        <v>128</v>
+      </c>
+      <c r="B130">
+        <v>1236</v>
+      </c>
+      <c r="C130" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="5">
+        <v>129</v>
+      </c>
+      <c r="B131">
+        <v>1236</v>
+      </c>
+      <c r="C131" t="s">
+        <v>6</v>
+      </c>
+      <c r="D131">
+        <v>3</v>
+      </c>
+      <c r="E131" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="5">
+        <v>130</v>
+      </c>
+      <c r="B132">
+        <v>1236</v>
+      </c>
+      <c r="C132" t="s">
+        <v>4</v>
+      </c>
+      <c r="D132">
+        <v>3</v>
+      </c>
+      <c r="E132" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A133" s="5">
+        <v>131</v>
+      </c>
+      <c r="B133">
+        <v>1236</v>
+      </c>
+      <c r="C133" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="5">
+        <v>132</v>
+      </c>
+      <c r="B134">
+        <v>1238</v>
+      </c>
+      <c r="C134" t="s">
+        <v>7</v>
+      </c>
+      <c r="D134">
+        <v>3</v>
+      </c>
+      <c r="E134" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="5">
+        <v>133</v>
+      </c>
+      <c r="B135">
+        <v>1238</v>
+      </c>
+      <c r="C135" t="s">
+        <v>6</v>
+      </c>
+      <c r="D135">
+        <v>3</v>
+      </c>
+      <c r="E135" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="5">
+        <v>134</v>
+      </c>
+      <c r="B136">
+        <v>1238</v>
+      </c>
+      <c r="C136" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="5">
+        <v>135</v>
+      </c>
+      <c r="B137">
+        <v>1238</v>
+      </c>
+      <c r="C137" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A138" s="5">
+        <v>136</v>
+      </c>
+      <c r="B138">
+        <v>1244</v>
+      </c>
+      <c r="C138" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A139" s="5">
+        <v>137</v>
+      </c>
+      <c r="B139">
+        <v>1244</v>
+      </c>
+      <c r="C139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="5">
+        <v>138</v>
+      </c>
+      <c r="B140">
+        <v>1244</v>
+      </c>
+      <c r="C140" t="s">
+        <v>4</v>
+      </c>
+      <c r="D140">
+        <v>3</v>
+      </c>
+      <c r="E140" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A141" s="5">
+        <v>139</v>
+      </c>
+      <c r="B141">
+        <v>1244</v>
+      </c>
+      <c r="C141" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A142" s="5">
+        <v>140</v>
+      </c>
+      <c r="B142">
+        <v>1269</v>
+      </c>
+      <c r="C142" t="s">
+        <v>7</v>
+      </c>
+      <c r="D142">
+        <v>3.25</v>
+      </c>
+      <c r="E142" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" s="5">
+        <v>141</v>
+      </c>
+      <c r="B143">
+        <v>1269</v>
+      </c>
+      <c r="C143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" s="5">
+        <v>142</v>
+      </c>
+      <c r="B144">
+        <v>1269</v>
+      </c>
+      <c r="C144" t="s">
+        <v>4</v>
+      </c>
+      <c r="D144">
+        <v>3</v>
+      </c>
+      <c r="E144" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="5">
+        <v>143</v>
+      </c>
+      <c r="B145">
+        <v>1269</v>
+      </c>
+      <c r="C145" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add mne pipeline, generated box plots and cluster maps
</commit_message>
<xml_diff>
--- a/xlsxs/animal-to-bestdepth.xlsx
+++ b/xlsxs/animal-to-bestdepth.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\MarshMountainSort\xlsxs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947A9260-655F-46D5-A25B-EEFDC3984105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695AE407-F872-4C5D-8892-177B503F4D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9167,8 +9167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>